<commit_message>
added some attacks to the charts for heroes
</commit_message>
<xml_diff>
--- a/Files as of 5-26/SpecialAttacks.xlsx
+++ b/Files as of 5-26/SpecialAttacks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sierra\Documents\Post Bacc College Stuff\CSCD 349\Team Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\CSCD349_TeamProject\Files as of 5-26\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Good Guys</t>
   </si>
@@ -90,6 +90,33 @@
   </si>
   <si>
     <t>Zombie</t>
+  </si>
+  <si>
+    <t>PerciseHit</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Bats</t>
+  </si>
+  <si>
+    <t>DoubleAttack</t>
+  </si>
+  <si>
+    <t>FireBall</t>
+  </si>
+  <si>
+    <t>ShieldBash</t>
+  </si>
+  <si>
+    <t>PoisonAttack</t>
+  </si>
+  <si>
+    <t>DrainLife</t>
+  </si>
+  <si>
+    <t>BodySlam</t>
   </si>
 </sst>
 </file>
@@ -419,7 +446,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,40 +485,67 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>